<commit_message>
Added AJAX request to load images from folder
</commit_message>
<xml_diff>
--- a/loading/svgCirclPoints.xlsx
+++ b/loading/svgCirclPoints.xlsx
@@ -53,6 +53,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -74,6 +75,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -155,12 +157,12 @@
   <dimension ref="B7:J22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="116" zoomScaleNormal="116" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.9591836734694"/>
   </cols>
   <sheetData>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>